<commit_message>
I make the Sales Mangment Part
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -4,26 +4,41 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -43,16 +58,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -409,221 +441,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="38.76" customWidth="1" style="1" min="1" max="1"/>
+    <col width="27.5" customWidth="1" style="1" min="2" max="2"/>
+    <col width="24.59" customWidth="1" style="1" min="3" max="3"/>
+    <col width="23.06" customWidth="1" style="1" min="4" max="4"/>
+    <col width="18.2" customWidth="1" style="1" min="5" max="5"/>
+    <col width="19.04" customWidth="1" style="1" min="6" max="6"/>
+    <col width="24.45" customWidth="1" style="1" min="7" max="7"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Iphon</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Charger</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="1" t="n">
         <v>3000</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>20:12:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="2">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>2024-09-03</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>15:41:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Master</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>18:08:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="2">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Adata</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Flash USB</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>64 GB</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>2400</v>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>17:33:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="2">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>MOBLIS</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>SIM Card</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>16:05:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="2">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>ooredoo</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>SIM Card</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>90</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-09-03</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>18:08:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Mstar MX-623</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Headphone</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="D6" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>19:43:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="2">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>GFUZ</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Charger</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>Micro USB</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>17:22:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="2">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Charger</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>Micro USB</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>17:34:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>djezzi</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>SIM Card</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E4" t="n">
-        <v>500</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-09-04</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>01:44:47</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Adata</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Flash USB</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>8 GB</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2400</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-09-04</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>02:27:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>MOBLIS</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SIM Card</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-09-04</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>01:28:16</t>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t>18:26:37</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I add return functionality in the sales part
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1000</v>
@@ -582,19 +582,19 @@
         </is>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>2400</v>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>2024-09-07</t>
+          <t>2024-09-09</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>17:33:16</t>
+          <t>21:40:23</t>
         </is>
       </c>
     </row>
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
I add fun to reset fileds when i switch from one to anther
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1000</v>
@@ -634,40 +634,40 @@
     <row r="6" ht="15" customHeight="1" s="2">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>ooredoo</t>
+          <t>GFUZ</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>SIM Card</t>
+          <t>Charger</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Micro USB</t>
         </is>
       </c>
       <c r="D6" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>2024-09-04</t>
+          <t>2024-09-07</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>19:43:03</t>
+          <t>17:22:39</t>
         </is>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="2">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>GFUZ</t>
+          <t>SAMSUNG</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -681,10 +681,10 @@
         </is>
       </c>
       <c r="D7" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
@@ -693,31 +693,31 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>17:22:39</t>
+          <t>17:34:00</t>
         </is>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="2">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>SAMSUNG</t>
+          <t>djezzi</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Charger</t>
+          <t>SIM Card</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>Micro USB</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1" t="inlineStr">
         <is>
@@ -726,40 +726,172 @@
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>17:34:00</t>
+          <t>18:26:37</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>djezzi</t>
+          <t>LDNIO</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
+          <t>Cable</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>Type C</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t>21:53:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>OOREDOO</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
           <t>SIM Card</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="C10" s="1" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="G10" s="1" t="inlineStr">
+        <is>
+          <t>21:59:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>jixsjixs</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>Cable</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>iPhone</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="inlineStr">
-        <is>
-          <t>2024-09-07</t>
-        </is>
-      </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t>18:26:37</t>
+      <c r="E11" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="G11" s="1" t="inlineStr">
+        <is>
+          <t>16:08:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>,ksx,ks,</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Car Charger</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Bluetooth</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>16:11:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>kxjoskxs</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Cable</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>iPhone</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>16:15:14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
I made GUI of  The Beverage section
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -655,12 +655,12 @@
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>2024-09-07</t>
+          <t>2024-09-12</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>17:22:39</t>
+          <t>13:40:58</t>
         </is>
       </c>
     </row>
@@ -863,33 +863,33 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>kxjoskxs</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="1" t="inlineStr">
         <is>
           <t>Cable</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="1" t="inlineStr">
         <is>
           <t>iPhone</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="1" t="inlineStr">
         <is>
           <t>2024-09-11</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="1" t="inlineStr">
         <is>
           <t>16:15:14</t>
         </is>

</xml_diff>